<commit_message>
using prov-indi fixed effect on CHARLS
now, using province as custom individual fixed effect on CHARLS dataset; later, applying the same settings on NHSS; and, a new quaratic term of income (AVGINDIINCOME_EARN2) is added to CHARLS, also, will be added to NHSS later.
</commit_message>
<xml_diff>
--- a/output/proc_1_CHARLS/PCAloading_CHARLS.xlsx
+++ b/output/proc_1_CHARLS/PCAloading_CHARLS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -27,6 +27,12 @@
     <t xml:space="preserve">RC3</t>
   </si>
   <si>
+    <t xml:space="preserve">RC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC5</t>
+  </si>
+  <si>
     <t xml:space="preserve">RC4</t>
   </si>
   <si>
@@ -39,9 +45,6 @@
     <t xml:space="preserve">MARITAL_AVELEN</t>
   </si>
   <si>
-    <t xml:space="preserve">AVGBMI</t>
-  </si>
-  <si>
     <t xml:space="preserve">DRINK1Y_RATIO</t>
   </si>
   <si>
@@ -75,15 +78,18 @@
     <t xml:space="preserve">JOBSTATUS_AGRI_RATIO</t>
   </si>
   <si>
+    <t xml:space="preserve">JOBSTATUS_NAGE_RATIO</t>
+  </si>
+  <si>
     <t xml:space="preserve">JOBSTATUS_NEWK_RATIO</t>
   </si>
   <si>
+    <t xml:space="preserve">RC7</t>
+  </si>
+  <si>
     <t xml:space="preserve">MARITAL_RATIO</t>
   </si>
   <si>
-    <t xml:space="preserve">SMOKEEVER_RATIO</t>
-  </si>
-  <si>
     <t xml:space="preserve">AVGEXP1W_FOOD</t>
   </si>
   <si>
@@ -94,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">CHILDLVNEAR_RATIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOBSTATUS_NAGE_RATIO</t>
   </si>
   <si>
     <t xml:space="preserve">JOBSTATUS_NAGS_RATIO</t>
@@ -450,277 +453,379 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.813055683070542</v>
+        <v>0.88718668615851</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.165776700683593</v>
+        <v>-0.144144988547339</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.10221255509623</v>
+        <v>-0.0571651818782883</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.159745415274498</v>
+        <v>-0.148681919740619</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0460349452946635</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-0.0286893866487868</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0975607467702275</v>
+        <v>-0.163093369845616</v>
       </c>
       <c r="C3" t="n">
-        <v>0.146116708242766</v>
+        <v>0.164768396646038</v>
       </c>
       <c r="D3" t="n">
-        <v>0.32444379446804</v>
+        <v>0.0253606416552824</v>
       </c>
       <c r="E3" t="n">
-        <v>0.452666591981311</v>
+        <v>0.245646139327318</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.102046735919805</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.612912368676942</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.90914979440795</v>
+        <v>0.930741143462427</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0446986276746422</v>
+        <v>0.120078329350535</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.097194615701928</v>
+        <v>-0.0526608527245032</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0561929105231327</v>
+        <v>0.113640708187669</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0609799315767796</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.0335123295361416</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.256119210961952</v>
+        <v>0.0794150467068352</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.670857137311829</v>
+        <v>-0.0709735050028291</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0692864768540159</v>
+        <v>0.0604687726386141</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0779962042804519</v>
+        <v>-0.0575069154848589</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.00674016334467371</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.763223249645825</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.100959852800323</v>
+        <v>-0.0355656539824122</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.17802451131341</v>
+        <v>0.0815696890053038</v>
       </c>
       <c r="D6" t="n">
-        <v>0.45987210550231</v>
+        <v>-0.0906592121399536</v>
       </c>
       <c r="E6" t="n">
-        <v>0.273000890756585</v>
+        <v>0.928449895532468</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.144927736996376</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0563140753271835</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.0367509252863239</v>
+        <v>0.0479137590231844</v>
       </c>
       <c r="C7" t="n">
-        <v>0.201930507092875</v>
+        <v>-0.00734072568255442</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.131912985187512</v>
+        <v>-0.0306017081763378</v>
       </c>
       <c r="E7" t="n">
-        <v>0.888965355059724</v>
+        <v>0.951871197755935</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.0354345643975689</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0802341687121033</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0602348768384489</v>
+        <v>0.180016096356673</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0908285965189283</v>
+        <v>-0.206459834489431</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0806787136484562</v>
+        <v>-0.0117083748859195</v>
       </c>
       <c r="E8" t="n">
-        <v>0.898210345318678</v>
+        <v>-0.0648150835681795</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.679902686199386</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0323152739056778</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.291604910094466</v>
+        <v>0.0318785630994733</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.601312893404358</v>
+        <v>0.0936566498714934</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0915680479831486</v>
+        <v>-0.0115961193886837</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0368446192453247</v>
+        <v>0.0301634741773827</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.728047200041228</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-0.0997849498157468</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>0.241714682848292</v>
+        <v>0.00897058717442542</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.301433823095384</v>
+        <v>0.050609554446579</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0239773524119679</v>
+        <v>0.957087527339415</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0385827626263673</v>
+        <v>-0.0638350540379625</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.0432722050686113</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0945630241064365</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0299180468841065</v>
+        <v>0.00958883801332884</v>
       </c>
       <c r="C11" t="n">
-        <v>0.112126858777587</v>
+        <v>0.143174876751917</v>
       </c>
       <c r="D11" t="n">
-        <v>0.862613480531085</v>
+        <v>0.947272538245271</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.142216824646627</v>
+        <v>-0.0555402268699357</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.043161672239431</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0874040327412882</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0119551386202717</v>
+        <v>0.0435693952903351</v>
       </c>
       <c r="C12" t="n">
-        <v>0.183767582593385</v>
+        <v>-0.241081955484789</v>
       </c>
       <c r="D12" t="n">
-        <v>0.858687108602435</v>
+        <v>-0.071280050443506</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.142409044889829</v>
+        <v>-0.200369904330724</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.648817264968937</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.103016683051024</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>0.195145600749666</v>
+        <v>0.758819220050551</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.524749226905983</v>
+        <v>0.270101419135645</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0319564620203368</v>
+        <v>0.124923517222997</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.161036415348934</v>
+        <v>0.0322916752291758</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.167544734891192</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.130969425481883</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>0.817795578266751</v>
+        <v>-0.069856165992134</v>
       </c>
       <c r="C14" t="n">
-        <v>0.115730703977624</v>
+        <v>0.779456164044369</v>
       </c>
       <c r="D14" t="n">
-        <v>0.168000285748132</v>
+        <v>0.213636888848949</v>
       </c>
       <c r="E14" t="n">
-        <v>0.00629203955655455</v>
+        <v>0.109250322441981</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.212614379271422</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.318114888851527</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0805063858397244</v>
+        <v>0.0672251437783013</v>
       </c>
       <c r="C15" t="n">
-        <v>0.806067758741376</v>
+        <v>0.947225263339962</v>
       </c>
       <c r="D15" t="n">
-        <v>0.341878115718485</v>
+        <v>0.152475040575057</v>
       </c>
       <c r="E15" t="n">
-        <v>0.123780933008402</v>
+        <v>0.064262085817992</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.147910484001572</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.114396252801658</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>0.205583871038156</v>
+        <v>-0.210027159120502</v>
       </c>
       <c r="C16" t="n">
-        <v>0.820675798779866</v>
+        <v>-0.779392327791553</v>
       </c>
       <c r="D16" t="n">
-        <v>0.252685207588993</v>
+        <v>0.0726500630155932</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0441009371537487</v>
+        <v>0.0465349959475207</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0146864981041822</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.244495733004015</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.479119852529362</v>
+        <v>-0.386805586205041</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0757398137307667</v>
+        <v>-0.0524865907743857</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.416948740745545</v>
+        <v>-0.208758746015093</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.159555247482724</v>
+        <v>-0.0356960506666224</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.220967106897498</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.507550045905446</v>
       </c>
     </row>
   </sheetData>
@@ -742,305 +847,467 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.322889260687019</v>
+        <v>-0.214572231784796</v>
       </c>
       <c r="C2" t="n">
-        <v>0.278549586739581</v>
+        <v>0.881108400901217</v>
       </c>
       <c r="D2" t="n">
-        <v>0.35378766965566</v>
+        <v>0.067128881153954</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.578388355290071</v>
+        <v>0.0786309094527856</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.0063294957543317</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.102377302889804</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.0350045235121683</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.132461289419203</v>
+        <v>-0.152296773250094</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.228386017837192</v>
+        <v>-0.43800797031574</v>
       </c>
       <c r="D3" t="n">
-        <v>0.241313036982982</v>
+        <v>-0.328374822283223</v>
       </c>
       <c r="E3" t="n">
-        <v>0.638026761853816</v>
+        <v>0.19569244420252</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.394604255628119</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.186753371792834</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.215523809034415</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.255060807340518</v>
+        <v>-0.156015839138029</v>
       </c>
       <c r="C4" t="n">
-        <v>0.162116240641049</v>
+        <v>0.870614015687656</v>
       </c>
       <c r="D4" t="n">
-        <v>0.534634367117096</v>
+        <v>-0.0072944306420246</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.628318910186002</v>
+        <v>-0.144258071326179</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0626276126006858</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0762957496917967</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.151527414268612</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.392946758847825</v>
+        <v>-0.283644410122958</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0983724809903564</v>
+        <v>-0.0657558626303956</v>
       </c>
       <c r="D5" t="n">
-        <v>0.30333584077791</v>
+        <v>0.00668946257008363</v>
       </c>
       <c r="E5" t="n">
-        <v>0.430386957349765</v>
+        <v>0.0926256933469915</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.723740459576101</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.0122085196940393</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-0.1154621832565</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.0880128619327183</v>
+        <v>0.104170197571148</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.232008601659188</v>
+        <v>0.253436966881592</v>
       </c>
       <c r="D6" t="n">
-        <v>0.64451108056328</v>
+        <v>0.316469527961999</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0728948104407568</v>
+        <v>0.166254590818565</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.142943174497681</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.561661752196503</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.0350414706084805</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>0.062283888210726</v>
+        <v>-0.108941152697723</v>
       </c>
       <c r="C7" t="n">
-        <v>0.57347010616038</v>
+        <v>-0.0277582912661303</v>
       </c>
       <c r="D7" t="n">
-        <v>0.242729268296572</v>
+        <v>0.102788158984461</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0299742524957248</v>
+        <v>-0.0953617522070969</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.0570145247764505</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.787282105115894</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.144097889752298</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0708890846222489</v>
+        <v>0.00227573677433688</v>
       </c>
       <c r="C8" t="n">
-        <v>0.325921168407459</v>
+        <v>0.0675031973532076</v>
       </c>
       <c r="D8" t="n">
-        <v>0.140501312288702</v>
+        <v>0.936090234045014</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0457111847280037</v>
+        <v>-0.0116966668774625</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0353391438933072</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.102811156286432</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.014725397531182</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0148907865269924</v>
+        <v>0.031985748372781</v>
       </c>
       <c r="C9" t="n">
-        <v>0.873154500823638</v>
+        <v>0.0370704985268565</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.117342745267571</v>
+        <v>0.912674793658593</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0670008760979504</v>
+        <v>0.1525899813309</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0582794745938844</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.197210696644722</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.00494057001429787</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0439877275281499</v>
+        <v>0.955148722884666</v>
       </c>
       <c r="C10" t="n">
-        <v>0.913463779659814</v>
+        <v>-0.107951608566766</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.103445423250767</v>
+        <v>-0.0513618660769178</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0516440558468895</v>
+        <v>0.0988477681041689</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.0629413776774466</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0201977938821569</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.0128076411765843</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n">
-        <v>0.956761883306599</v>
+        <v>0.724296648523608</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0284102779716096</v>
+        <v>-0.223727428297577</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0318040266440653</v>
+        <v>0.27993235114076</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0831831602841165</v>
+        <v>-0.10258985720099</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.21595193209955</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.117890758278472</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0216074125642645</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n">
-        <v>0.760274996759195</v>
+        <v>0.948915846579949</v>
       </c>
       <c r="C12" t="n">
-        <v>0.152535258916064</v>
+        <v>-0.139747210908952</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.290285686338219</v>
+        <v>-0.0570955495889937</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0439300645356495</v>
+        <v>0.084751059175772</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-0.07844367712414</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.00730817980701672</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-0.00537835625436425</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>0.956805253046544</v>
+        <v>-0.20215214060006</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0471085454289299</v>
+        <v>0.639065983783579</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00784755724962132</v>
+        <v>0.0789068265441356</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0914136960441654</v>
+        <v>-0.241869439669255</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.264256328763045</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0540489520722349</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.331949611169065</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.277657549360386</v>
+        <v>0.0218916442688938</v>
       </c>
       <c r="C14" t="n">
-        <v>0.182965810501126</v>
+        <v>-0.164950990902395</v>
       </c>
       <c r="D14" t="n">
-        <v>0.637844876091906</v>
+        <v>-0.109493700455018</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.401518091446564</v>
+        <v>-0.594590694266201</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.303677130427794</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-0.407088393031316</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.391703351277459</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>0.11236395571196</v>
+        <v>0.138387401196175</v>
       </c>
       <c r="C15" t="n">
-        <v>0.247560322112641</v>
+        <v>-0.139499436729902</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0471385198339845</v>
+        <v>0.0787819660918628</v>
       </c>
       <c r="E15" t="n">
-        <v>0.577680531386776</v>
+        <v>0.763958979290977</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.181999842230487</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0211806240751871</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-0.108427153227375</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.0237456507199604</v>
+        <v>-0.0906185106024216</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.021011553371807</v>
+        <v>-0.222854052885237</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.11068966688676</v>
+        <v>0.0254798753576386</v>
       </c>
       <c r="E16" t="n">
-        <v>0.454823627193267</v>
+        <v>0.604080761605345</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.0895121511274372</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.356329096946963</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.425951113393035</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.0746675381271638</v>
+        <v>-0.037087153970814</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.0607257275634399</v>
+        <v>-0.21120690286187</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.505128214687832</v>
+        <v>0.00182614128114163</v>
       </c>
       <c r="E17" t="n">
-        <v>0.117787250565962</v>
+        <v>0.0694103995295483</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.0347393100437785</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.133907085996241</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-0.783306632942868</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B18" t="n">
-        <v>0.133188135052567</v>
+        <v>-0.00975696020297295</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.279149892109125</v>
+        <v>-0.321287575883903</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.574299230555142</v>
+        <v>-0.142109232792578</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.0655139246916441</v>
+        <v>0.0629282736389248</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.698505076857583</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.00124768421458535</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-0.18444909446362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>